<commit_message>
Quase Acabando o Deploy! Graças a Deus! - 13/01 - Leo
</commit_message>
<xml_diff>
--- a/Credit_Policy/cubo_rating.xlsx
+++ b/Credit_Policy/cubo_rating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leova\Desktop\Projetos\05_modelo_risco_de_credito\Credit_Policy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD51BBB-4FC8-4053-A129-6D659AD1E2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BF6C2E-F775-40A4-A192-93780A86FD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="19200" windowWidth="16200" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="16200" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>rating_model</t>
   </si>
@@ -368,12 +368,6 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -383,13 +377,271 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="70">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -1187,6 +1439,612 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CBA5859F-A714-468C-BB53-A03F2D9B0C40}" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Rating Modelo" colHeaderCaption="Rating Política">
+  <location ref="A32:L44" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Swap-in | Swap Out" fld="2" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <formats count="35">
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="7"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="0"/>
+          <reference field="1" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="9">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="8">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="6">
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="6">
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="5">
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="4">
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="3">
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="2">
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="24">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="8" selected="0">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="7">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="6">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="5">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="4">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="4">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="2">
+            <x v="2"/>
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <conditionalFormats count="1">
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="10">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+            <reference field="1" count="10" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F122F887-D27A-4C25-A17F-E3C22A275442}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Rating Modelo" colHeaderCaption="Rating Política">
   <location ref="A3:L15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
@@ -1302,7 +2160,7 @@
     <dataField name="Swap-in | Swap Out" fld="2" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <formats count="35">
-    <format dxfId="34">
+    <format dxfId="69">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1314,7 +2172,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="68">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1326,7 +2184,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="67">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1338,7 +2196,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="66">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1350,7 +2208,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="65">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1362,7 +2220,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="64">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1374,7 +2232,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="63">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1386,7 +2244,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="62">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1398,7 +2256,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="61">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1410,16 +2268,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="60">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="59">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="58">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="57">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -1427,7 +2285,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="56">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="9">
@@ -1447,7 +2305,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="55">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="8">
@@ -1466,7 +2324,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="54">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="6">
@@ -1483,7 +2341,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="53">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1495,7 +2353,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="52">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="6">
@@ -1512,7 +2370,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="51">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="5">
@@ -1528,7 +2386,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="50">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="4">
@@ -1543,7 +2401,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="49">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="3">
@@ -1557,7 +2415,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="48">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="2">
@@ -1570,7 +2428,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="47">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1582,7 +2440,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="46">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1594,7 +2452,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="45">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="2">
@@ -1614,7 +2472,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="44">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="7">
@@ -1632,7 +2490,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="43">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="6">
@@ -1649,7 +2507,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="42">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="5">
@@ -1665,7 +2523,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="41">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="4">
@@ -1680,7 +2538,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="40">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="4">
@@ -1695,7 +2553,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="39">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="2">
@@ -1708,7 +2566,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="38">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1720,14 +2578,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="37">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="36">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1739,7 +2597,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="35">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -2040,10 +2898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B81726-F8C5-4B98-B37C-017D2DB08893}">
-  <dimension ref="A1:AH20"/>
+  <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="M12" workbookViewId="0">
+      <selection activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,20 +2946,20 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="W3" s="23" t="s">
+      <c r="W3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="23"/>
-      <c r="AH3" s="23"/>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="26"/>
+      <c r="AA3" s="26"/>
+      <c r="AB3" s="26"/>
+      <c r="AC3" s="26"/>
+      <c r="AD3" s="26"/>
+      <c r="AE3" s="26"/>
+      <c r="AF3" s="26"/>
+      <c r="AG3" s="26"/>
+      <c r="AH3" s="26"/>
     </row>
     <row r="4" spans="1:34" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -2140,7 +2998,7 @@
       <c r="L4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="W4" s="24" t="s">
+      <c r="W4" s="27" t="s">
         <v>5</v>
       </c>
       <c r="Y4" s="18">
@@ -2211,7 +3069,7 @@
       <c r="L5" s="8">
         <v>0.10000321691669257</v>
       </c>
-      <c r="W5" s="24"/>
+      <c r="W5" s="27"/>
       <c r="X5" s="13">
         <v>0</v>
       </c>
@@ -2283,7 +3141,7 @@
       <c r="L6" s="8">
         <v>0.10000321691669257</v>
       </c>
-      <c r="W6" s="24"/>
+      <c r="W6" s="27"/>
       <c r="X6" s="14">
         <v>1</v>
       </c>
@@ -2355,7 +3213,7 @@
       <c r="L7" s="8">
         <v>9.9992493861050649E-2</v>
       </c>
-      <c r="W7" s="24"/>
+      <c r="W7" s="27"/>
       <c r="X7" s="14">
         <v>2</v>
       </c>
@@ -2427,7 +3285,7 @@
       <c r="L8" s="8">
         <v>0.10000321691669257</v>
       </c>
-      <c r="W8" s="24"/>
+      <c r="W8" s="27"/>
       <c r="X8" s="14">
         <v>3</v>
       </c>
@@ -2499,7 +3357,7 @@
       <c r="L9" s="8">
         <v>9.9992493861050649E-2</v>
       </c>
-      <c r="W9" s="24"/>
+      <c r="W9" s="27"/>
       <c r="X9" s="14">
         <v>4</v>
       </c>
@@ -2571,7 +3429,7 @@
       <c r="L10" s="8">
         <v>0.10000321691669257</v>
       </c>
-      <c r="W10" s="24"/>
+      <c r="W10" s="27"/>
       <c r="X10" s="14">
         <v>5</v>
       </c>
@@ -2643,17 +3501,17 @@
       <c r="L11" s="8">
         <v>0.10000321691669257</v>
       </c>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25" t="s">
+      <c r="O11" s="23"/>
+      <c r="P11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="Q11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="R11" s="25" t="s">
+      <c r="R11" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="W11" s="24"/>
+      <c r="W11" s="27"/>
       <c r="X11" s="14">
         <v>6</v>
       </c>
@@ -2732,13 +3590,13 @@
         <f>SUM(C5:K5,D6:K6,E7:K7,F8:K8,G9:K9,H10:K10,I11:K11,J12:K12,GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",8,"rating_politica",9))</f>
         <v>0.3560697856461178</v>
       </c>
-      <c r="Q12" s="27">
+      <c r="Q12" s="25">
         <v>30232753</v>
       </c>
-      <c r="R12" s="25" t="s">
+      <c r="R12" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="W12" s="24"/>
+      <c r="W12" s="27"/>
       <c r="X12" s="14">
         <v>7</v>
       </c>
@@ -2817,13 +3675,13 @@
         <f>SUM(GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",0,"rating_politica",0),GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",1,"rating_politica",1),GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",2,"rating_politica",2),GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",3,"rating_politica",3),GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",4,"rating_politica",4),GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",5,"rating_politica",5),GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",6,"rating_politica",6),GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",7,"rating_politica",7),GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",8,"rating_politica",8),GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",9,"rating_politica",9))</f>
         <v>0.28015055170121278</v>
       </c>
-      <c r="Q13" s="27">
+      <c r="Q13" s="25">
         <v>51387058</v>
       </c>
-      <c r="R13" s="25" t="s">
+      <c r="R13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="W13" s="24"/>
+      <c r="W13" s="27"/>
       <c r="X13" s="14">
         <v>8</v>
       </c>
@@ -2902,13 +3760,13 @@
         <f>SUM(B14:J14,B13:I13,B12:H12,B11:G11,B10:F10,B9:E9,B8:D8,B7:C7,GETPIVOTDATA("mesmo_resultado",$A$3,"rating_model",1,"rating_politica",0))</f>
         <v>0.36377966265266959</v>
       </c>
-      <c r="Q14" s="27">
+      <c r="Q14" s="25">
         <v>128573551</v>
       </c>
-      <c r="R14" s="26" t="s">
+      <c r="R14" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="W14" s="24"/>
+      <c r="W14" s="27"/>
       <c r="X14" s="15">
         <v>9</v>
       </c>
@@ -2985,16 +3843,903 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="P20">
         <v>28</v>
       </c>
     </row>
+    <row r="32" spans="1:34" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="W32" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="X32" s="26"/>
+      <c r="Y32" s="26"/>
+      <c r="Z32" s="26"/>
+      <c r="AA32" s="26"/>
+      <c r="AB32" s="26"/>
+      <c r="AC32" s="26"/>
+      <c r="AD32" s="26"/>
+      <c r="AE32" s="26"/>
+      <c r="AF32" s="26"/>
+      <c r="AG32" s="26"/>
+      <c r="AH32" s="26"/>
+    </row>
+    <row r="33" spans="1:34" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4">
+        <v>3</v>
+      </c>
+      <c r="F33" s="4">
+        <v>4</v>
+      </c>
+      <c r="G33" s="4">
+        <v>5</v>
+      </c>
+      <c r="H33" s="4">
+        <v>6</v>
+      </c>
+      <c r="I33" s="4">
+        <v>7</v>
+      </c>
+      <c r="J33" s="4">
+        <v>8</v>
+      </c>
+      <c r="K33" s="4">
+        <v>9</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W33" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y33" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="19">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="19">
+        <v>2</v>
+      </c>
+      <c r="AB33" s="19">
+        <v>3</v>
+      </c>
+      <c r="AC33" s="19">
+        <v>4</v>
+      </c>
+      <c r="AD33" s="19">
+        <v>5</v>
+      </c>
+      <c r="AE33" s="19">
+        <v>6</v>
+      </c>
+      <c r="AF33" s="19">
+        <v>7</v>
+      </c>
+      <c r="AG33" s="19">
+        <v>8</v>
+      </c>
+      <c r="AH33" s="20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>0</v>
+      </c>
+      <c r="B34" s="6">
+        <v>5.0795114575849537E-2</v>
+      </c>
+      <c r="C34" s="7">
+        <v>2.338698435506182E-2</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1.3736234277319665E-2</v>
+      </c>
+      <c r="E34" s="7">
+        <v>7.0772167236775796E-3</v>
+      </c>
+      <c r="F34" s="7">
+        <v>2.4663027976452169E-3</v>
+      </c>
+      <c r="G34" s="7">
+        <v>9.4362889649034394E-4</v>
+      </c>
+      <c r="H34" s="7">
+        <v>7.2916778365162934E-4</v>
+      </c>
+      <c r="I34" s="7">
+        <v>4.1819917003549329E-4</v>
+      </c>
+      <c r="J34" s="7">
+        <v>3.8603000310968616E-4</v>
+      </c>
+      <c r="K34" s="7">
+        <v>6.4338333851614356E-5</v>
+      </c>
+      <c r="L34" s="8">
+        <v>0.10000321691669257</v>
+      </c>
+      <c r="W34" s="27"/>
+      <c r="X34" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="16">
+        <v>5.0795114575849537E-2</v>
+      </c>
+      <c r="Z34" s="17">
+        <v>2.338698435506182E-2</v>
+      </c>
+      <c r="AA34" s="17">
+        <v>1.3736234277319665E-2</v>
+      </c>
+      <c r="AB34" s="17">
+        <v>7.0772167236775796E-3</v>
+      </c>
+      <c r="AC34" s="17">
+        <v>2.4663027976452169E-3</v>
+      </c>
+      <c r="AD34" s="17">
+        <v>9.4362889649034394E-4</v>
+      </c>
+      <c r="AE34" s="17">
+        <v>7.2916778365162934E-4</v>
+      </c>
+      <c r="AF34" s="17">
+        <v>4.1819917003549329E-4</v>
+      </c>
+      <c r="AG34" s="17">
+        <v>3.8603000310968616E-4</v>
+      </c>
+      <c r="AH34" s="17">
+        <v>6.4338333851614356E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>1</v>
+      </c>
+      <c r="B35" s="9">
+        <v>2.6850531327407057E-2</v>
+      </c>
+      <c r="C35" s="6">
+        <v>2.5188457702907022E-2</v>
+      </c>
+      <c r="D35" s="7">
+        <v>1.9129931265213337E-2</v>
+      </c>
+      <c r="E35" s="7">
+        <v>1.4068649002219673E-2</v>
+      </c>
+      <c r="F35" s="7">
+        <v>8.85724396023891E-3</v>
+      </c>
+      <c r="G35" s="7">
+        <v>3.76379253031944E-3</v>
+      </c>
+      <c r="H35" s="7">
+        <v>1.3725511221677729E-3</v>
+      </c>
+      <c r="I35" s="7">
+        <v>5.3615278209678634E-4</v>
+      </c>
+      <c r="J35" s="7">
+        <v>2.037380571967788E-4</v>
+      </c>
+      <c r="K35" s="7">
+        <v>3.2169166925807178E-5</v>
+      </c>
+      <c r="L35" s="8">
+        <v>0.10000321691669257</v>
+      </c>
+      <c r="W35" s="27"/>
+      <c r="X35" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="12">
+        <v>2.6850531327407057E-2</v>
+      </c>
+      <c r="Z35" s="6">
+        <v>2.5188457702907022E-2</v>
+      </c>
+      <c r="AA35" s="7">
+        <v>1.9129931265213337E-2</v>
+      </c>
+      <c r="AB35" s="7">
+        <v>1.4068649002219673E-2</v>
+      </c>
+      <c r="AC35" s="7">
+        <v>8.85724396023891E-3</v>
+      </c>
+      <c r="AD35" s="7">
+        <v>3.76379253031944E-3</v>
+      </c>
+      <c r="AE35" s="7">
+        <v>1.3725511221677729E-3</v>
+      </c>
+      <c r="AF35" s="7">
+        <v>5.3615278209678634E-4</v>
+      </c>
+      <c r="AG35" s="7">
+        <v>2.037380571967788E-4</v>
+      </c>
+      <c r="AH35" s="7">
+        <v>3.2169166925807178E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>2</v>
+      </c>
+      <c r="B36" s="9">
+        <v>1.3435988719345465E-2</v>
+      </c>
+      <c r="C36" s="9">
+        <v>2.0320190441468201E-2</v>
+      </c>
+      <c r="D36" s="6">
+        <v>1.9837652937581093E-2</v>
+      </c>
+      <c r="E36" s="7">
+        <v>1.6459890410371339E-2</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1.3435988719345465E-2</v>
+      </c>
+      <c r="G36" s="7">
+        <v>9.3719506310518241E-3</v>
+      </c>
+      <c r="H36" s="7">
+        <v>4.857544205796884E-3</v>
+      </c>
+      <c r="I36" s="7">
+        <v>1.6942427914258447E-3</v>
+      </c>
+      <c r="J36" s="7">
+        <v>5.1470667081291485E-4</v>
+      </c>
+      <c r="K36" s="7">
+        <v>6.4338333851614356E-5</v>
+      </c>
+      <c r="L36" s="8">
+        <v>9.9992493861050649E-2</v>
+      </c>
+      <c r="W36" s="27"/>
+      <c r="X36" s="14">
+        <v>2</v>
+      </c>
+      <c r="Y36" s="12">
+        <v>1.3435988719345465E-2</v>
+      </c>
+      <c r="Z36" s="9">
+        <v>2.0320190441468201E-2</v>
+      </c>
+      <c r="AA36" s="6">
+        <v>1.9837652937581093E-2</v>
+      </c>
+      <c r="AB36" s="7">
+        <v>1.6459890410371339E-2</v>
+      </c>
+      <c r="AC36" s="7">
+        <v>1.3435988719345465E-2</v>
+      </c>
+      <c r="AD36" s="7">
+        <v>9.3719506310518241E-3</v>
+      </c>
+      <c r="AE36" s="7">
+        <v>4.857544205796884E-3</v>
+      </c>
+      <c r="AF36" s="7">
+        <v>1.6942427914258447E-3</v>
+      </c>
+      <c r="AG36" s="7">
+        <v>5.1470667081291485E-4</v>
+      </c>
+      <c r="AH36" s="7">
+        <v>6.4338333851614356E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>3</v>
+      </c>
+      <c r="B37" s="9">
+        <v>6.2300953279646569E-3</v>
+      </c>
+      <c r="C37" s="9">
+        <v>1.5344692623610023E-2</v>
+      </c>
+      <c r="D37" s="9">
+        <v>1.7017489303751996E-2</v>
+      </c>
+      <c r="E37" s="6">
+        <v>1.558059984773261E-2</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1.6545674855506825E-2</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1.3607557609616436E-2</v>
+      </c>
+      <c r="H37" s="7">
+        <v>1.0004610913926033E-2</v>
+      </c>
+      <c r="I37" s="7">
+        <v>3.8174078085291183E-3</v>
+      </c>
+      <c r="J37" s="7">
+        <v>1.7156889027097162E-3</v>
+      </c>
+      <c r="K37" s="7">
+        <v>1.3939972334516443E-4</v>
+      </c>
+      <c r="L37" s="8">
+        <v>0.10000321691669257</v>
+      </c>
+      <c r="W37" s="27"/>
+      <c r="X37" s="14">
+        <v>3</v>
+      </c>
+      <c r="Y37" s="12">
+        <v>6.2300953279646569E-3</v>
+      </c>
+      <c r="Z37" s="9">
+        <v>1.5344692623610023E-2</v>
+      </c>
+      <c r="AA37" s="9">
+        <v>1.7017489303751996E-2</v>
+      </c>
+      <c r="AB37" s="6">
+        <v>1.558059984773261E-2</v>
+      </c>
+      <c r="AC37" s="7">
+        <v>1.6545674855506825E-2</v>
+      </c>
+      <c r="AD37" s="7">
+        <v>1.3607557609616436E-2</v>
+      </c>
+      <c r="AE37" s="7">
+        <v>1.0004610913926033E-2</v>
+      </c>
+      <c r="AF37" s="7">
+        <v>3.8174078085291183E-3</v>
+      </c>
+      <c r="AG37" s="7">
+        <v>1.7156889027097162E-3</v>
+      </c>
+      <c r="AH37" s="7">
+        <v>1.3939972334516443E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>4</v>
+      </c>
+      <c r="B38" s="9">
+        <v>1.6727966801419732E-3</v>
+      </c>
+      <c r="C38" s="9">
+        <v>9.4362889649034394E-3</v>
+      </c>
+      <c r="D38" s="9">
+        <v>1.4508294283539037E-2</v>
+      </c>
+      <c r="E38" s="9">
+        <v>1.5634215125942288E-2</v>
+      </c>
+      <c r="F38" s="6">
+        <v>1.6953150969900382E-2</v>
+      </c>
+      <c r="G38" s="7">
+        <v>1.4218771781206773E-2</v>
+      </c>
+      <c r="H38" s="7">
+        <v>1.5634215125942288E-2</v>
+      </c>
+      <c r="I38" s="7">
+        <v>8.4712139571292231E-3</v>
+      </c>
+      <c r="J38" s="7">
+        <v>2.9810094684581318E-3</v>
+      </c>
+      <c r="K38" s="7">
+        <v>4.8253750388710766E-4</v>
+      </c>
+      <c r="L38" s="8">
+        <v>9.9992493861050649E-2</v>
+      </c>
+      <c r="W38" s="27"/>
+      <c r="X38" s="14">
+        <v>4</v>
+      </c>
+      <c r="Y38" s="12">
+        <v>1.6727966801419732E-3</v>
+      </c>
+      <c r="Z38" s="9">
+        <v>9.4362889649034394E-3</v>
+      </c>
+      <c r="AA38" s="9">
+        <v>1.4508294283539037E-2</v>
+      </c>
+      <c r="AB38" s="9">
+        <v>1.5634215125942288E-2</v>
+      </c>
+      <c r="AC38" s="6">
+        <v>1.6953150969900382E-2</v>
+      </c>
+      <c r="AD38" s="7">
+        <v>1.4218771781206773E-2</v>
+      </c>
+      <c r="AE38" s="7">
+        <v>1.5634215125942288E-2</v>
+      </c>
+      <c r="AF38" s="7">
+        <v>8.4712139571292231E-3</v>
+      </c>
+      <c r="AG38" s="7">
+        <v>2.9810094684581318E-3</v>
+      </c>
+      <c r="AH38" s="7">
+        <v>4.8253750388710766E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>5</v>
+      </c>
+      <c r="B39" s="9">
+        <v>6.7555250544195072E-4</v>
+      </c>
+      <c r="C39" s="9">
+        <v>4.4822372583291333E-3</v>
+      </c>
+      <c r="D39" s="9">
+        <v>9.2861661859163381E-3</v>
+      </c>
+      <c r="E39" s="9">
+        <v>1.4004310668368058E-2</v>
+      </c>
+      <c r="F39" s="9">
+        <v>1.6910258747332641E-2</v>
+      </c>
+      <c r="G39" s="6">
+        <v>1.5977352906484232E-2</v>
+      </c>
+      <c r="H39" s="7">
+        <v>1.6717243745777797E-2</v>
+      </c>
+      <c r="I39" s="7">
+        <v>1.4154433447355159E-2</v>
+      </c>
+      <c r="J39" s="7">
+        <v>6.8949247777646714E-3</v>
+      </c>
+      <c r="K39" s="7">
+        <v>9.0073667392260096E-4</v>
+      </c>
+      <c r="L39" s="8">
+        <v>0.10000321691669257</v>
+      </c>
+      <c r="W39" s="27"/>
+      <c r="X39" s="14">
+        <v>5</v>
+      </c>
+      <c r="Y39" s="12">
+        <v>6.7555250544195072E-4</v>
+      </c>
+      <c r="Z39" s="9">
+        <v>4.4822372583291333E-3</v>
+      </c>
+      <c r="AA39" s="9">
+        <v>9.2861661859163381E-3</v>
+      </c>
+      <c r="AB39" s="9">
+        <v>1.4004310668368058E-2</v>
+      </c>
+      <c r="AC39" s="9">
+        <v>1.6910258747332641E-2</v>
+      </c>
+      <c r="AD39" s="6">
+        <v>1.5977352906484232E-2</v>
+      </c>
+      <c r="AE39" s="7">
+        <v>1.6717243745777797E-2</v>
+      </c>
+      <c r="AF39" s="7">
+        <v>1.4154433447355159E-2</v>
+      </c>
+      <c r="AG39" s="7">
+        <v>6.8949247777646714E-3</v>
+      </c>
+      <c r="AH39" s="7">
+        <v>9.0073667392260096E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>6</v>
+      </c>
+      <c r="B40" s="9">
+        <v>3.0024555797420035E-4</v>
+      </c>
+      <c r="C40" s="9">
+        <v>1.4261664003774517E-3</v>
+      </c>
+      <c r="D40" s="9">
+        <v>5.0612822629936627E-3</v>
+      </c>
+      <c r="E40" s="9">
+        <v>1.048714841781314E-2</v>
+      </c>
+      <c r="F40" s="9">
+        <v>1.477637067458743E-2</v>
+      </c>
+      <c r="G40" s="9">
+        <v>1.7542919030206848E-2</v>
+      </c>
+      <c r="H40" s="6">
+        <v>1.736062708429394E-2</v>
+      </c>
+      <c r="I40" s="7">
+        <v>1.7993287367168147E-2</v>
+      </c>
+      <c r="J40" s="7">
+        <v>1.2449467600287378E-2</v>
+      </c>
+      <c r="K40" s="7">
+        <v>2.6057025209903816E-3</v>
+      </c>
+      <c r="L40" s="8">
+        <v>0.10000321691669257</v>
+      </c>
+      <c r="W40" s="27"/>
+      <c r="X40" s="14">
+        <v>6</v>
+      </c>
+      <c r="Y40" s="12">
+        <v>3.0024555797420035E-4</v>
+      </c>
+      <c r="Z40" s="9">
+        <v>1.4261664003774517E-3</v>
+      </c>
+      <c r="AA40" s="9">
+        <v>5.0612822629936627E-3</v>
+      </c>
+      <c r="AB40" s="9">
+        <v>1.048714841781314E-2</v>
+      </c>
+      <c r="AC40" s="9">
+        <v>1.477637067458743E-2</v>
+      </c>
+      <c r="AD40" s="9">
+        <v>1.7542919030206848E-2</v>
+      </c>
+      <c r="AE40" s="6">
+        <v>1.736062708429394E-2</v>
+      </c>
+      <c r="AF40" s="7">
+        <v>1.7993287367168147E-2</v>
+      </c>
+      <c r="AG40" s="7">
+        <v>1.2449467600287378E-2</v>
+      </c>
+      <c r="AH40" s="7">
+        <v>2.6057025209903816E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>7</v>
+      </c>
+      <c r="B41" s="9">
+        <v>0</v>
+      </c>
+      <c r="C41" s="9">
+        <v>3.0024555797420035E-4</v>
+      </c>
+      <c r="D41" s="9">
+        <v>1.3189358439580942E-3</v>
+      </c>
+      <c r="E41" s="9">
+        <v>5.1363436524872125E-3</v>
+      </c>
+      <c r="F41" s="9">
+        <v>7.9350611750324367E-3</v>
+      </c>
+      <c r="G41" s="9">
+        <v>1.5559153736448738E-2</v>
+      </c>
+      <c r="H41" s="9">
+        <v>1.7103273748887482E-2</v>
+      </c>
+      <c r="I41" s="6">
+        <v>2.3665783801752147E-2</v>
+      </c>
+      <c r="J41" s="7">
+        <v>2.0920681557416602E-2</v>
+      </c>
+      <c r="K41" s="7">
+        <v>8.0530147870937294E-3</v>
+      </c>
+      <c r="L41" s="8">
+        <v>9.9992493861050649E-2</v>
+      </c>
+      <c r="W41" s="27"/>
+      <c r="X41" s="14">
+        <v>7</v>
+      </c>
+      <c r="Y41" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="9">
+        <v>3.0024555797420035E-4</v>
+      </c>
+      <c r="AA41" s="9">
+        <v>1.3189358439580942E-3</v>
+      </c>
+      <c r="AB41" s="9">
+        <v>5.1363436524872125E-3</v>
+      </c>
+      <c r="AC41" s="9">
+        <v>7.9350611750324367E-3</v>
+      </c>
+      <c r="AD41" s="9">
+        <v>1.5559153736448738E-2</v>
+      </c>
+      <c r="AE41" s="9">
+        <v>1.7103273748887482E-2</v>
+      </c>
+      <c r="AF41" s="6">
+        <v>2.3665783801752147E-2</v>
+      </c>
+      <c r="AG41" s="7">
+        <v>2.0920681557416602E-2</v>
+      </c>
+      <c r="AH41" s="7">
+        <v>8.0530147870937294E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>8</v>
+      </c>
+      <c r="B42" s="9">
+        <v>0</v>
+      </c>
+      <c r="C42" s="9">
+        <v>4.2892222567742904E-5</v>
+      </c>
+      <c r="D42" s="9">
+        <v>1.0723055641935726E-4</v>
+      </c>
+      <c r="E42" s="9">
+        <v>9.4362889649034394E-4</v>
+      </c>
+      <c r="F42" s="9">
+        <v>2.4341336307194096E-3</v>
+      </c>
+      <c r="G42" s="9">
+        <v>7.4310775598614579E-3</v>
+      </c>
+      <c r="H42" s="9">
+        <v>1.2524528989780927E-2</v>
+      </c>
+      <c r="I42" s="9">
+        <v>2.1231650171032738E-2</v>
+      </c>
+      <c r="J42" s="6">
+        <v>3.1096861361613607E-2</v>
+      </c>
+      <c r="K42" s="7">
+        <v>2.4191213528206999E-2</v>
+      </c>
+      <c r="L42" s="8">
+        <v>0.10000321691669257</v>
+      </c>
+      <c r="W42" s="27"/>
+      <c r="X42" s="14">
+        <v>8</v>
+      </c>
+      <c r="Y42" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="9">
+        <v>4.2892222567742904E-5</v>
+      </c>
+      <c r="AA42" s="9">
+        <v>1.0723055641935726E-4</v>
+      </c>
+      <c r="AB42" s="9">
+        <v>9.4362889649034394E-4</v>
+      </c>
+      <c r="AC42" s="9">
+        <v>2.4341336307194096E-3</v>
+      </c>
+      <c r="AD42" s="9">
+        <v>7.4310775598614579E-3</v>
+      </c>
+      <c r="AE42" s="9">
+        <v>1.2524528989780927E-2</v>
+      </c>
+      <c r="AF42" s="9">
+        <v>2.1231650171032738E-2</v>
+      </c>
+      <c r="AG42" s="6">
+        <v>3.1096861361613607E-2</v>
+      </c>
+      <c r="AH42" s="7">
+        <v>2.4191213528206999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>9</v>
+      </c>
+      <c r="B43" s="9">
+        <v>0</v>
+      </c>
+      <c r="C43" s="9">
+        <v>1.0723055641935726E-5</v>
+      </c>
+      <c r="D43" s="9">
+        <v>0</v>
+      </c>
+      <c r="E43" s="9">
+        <v>4.2892222567742904E-5</v>
+      </c>
+      <c r="F43" s="9">
+        <v>2.2518416848065024E-4</v>
+      </c>
+      <c r="G43" s="9">
+        <v>1.5548430680806802E-3</v>
+      </c>
+      <c r="H43" s="9">
+        <v>3.6029466956904038E-3</v>
+      </c>
+      <c r="I43" s="9">
+        <v>8.2138606217227669E-3</v>
+      </c>
+      <c r="J43" s="9">
+        <v>2.2657816571410191E-2</v>
+      </c>
+      <c r="K43" s="6">
+        <v>6.3694950513098217E-2</v>
+      </c>
+      <c r="L43" s="8">
+        <v>0.10000321691669257</v>
+      </c>
+      <c r="W43" s="27"/>
+      <c r="X43" s="15">
+        <v>9</v>
+      </c>
+      <c r="Y43" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="9">
+        <v>1.0723055641935726E-5</v>
+      </c>
+      <c r="AA43" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="9">
+        <v>4.2892222567742904E-5</v>
+      </c>
+      <c r="AC43" s="9">
+        <v>2.2518416848065024E-4</v>
+      </c>
+      <c r="AD43" s="9">
+        <v>1.5548430680806802E-3</v>
+      </c>
+      <c r="AE43" s="9">
+        <v>3.6029466956904038E-3</v>
+      </c>
+      <c r="AF43" s="9">
+        <v>8.2138606217227669E-3</v>
+      </c>
+      <c r="AG43" s="9">
+        <v>2.2657816571410191E-2</v>
+      </c>
+      <c r="AH43" s="6">
+        <v>6.3694950513098217E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="5">
+        <v>9.9960324694124844E-2</v>
+      </c>
+      <c r="C44" s="5">
+        <v>9.9938878582840965E-2</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0.10000321691669257</v>
+      </c>
+      <c r="E44" s="5">
+        <v>9.9434894967669982E-2</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0.10053936969878936</v>
+      </c>
+      <c r="G44" s="5">
+        <v>9.997104774976677E-2</v>
+      </c>
+      <c r="H44" s="5">
+        <v>9.990670941591516E-2</v>
+      </c>
+      <c r="I44" s="5">
+        <v>0.10019623191824742</v>
+      </c>
+      <c r="J44" s="5">
+        <v>9.982092497077967E-2</v>
+      </c>
+      <c r="K44" s="5">
+        <v>0.10022840108517322</v>
+      </c>
+      <c r="L44" s="5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="W3:AH3"/>
     <mergeCell ref="W4:W14"/>
+    <mergeCell ref="W32:AH32"/>
+    <mergeCell ref="W33:W43"/>
   </mergeCells>
+  <conditionalFormatting pivot="1" sqref="B34:K43">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y34:AH43">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>